<commit_message>
Update Bill Of Materials (1).xlsx
</commit_message>
<xml_diff>
--- a/Excel Files/Bill Of Materials (1).xlsx
+++ b/Excel Files/Bill Of Materials (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himol\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himol\OneDrive\Documents\GitHub\EMGingers-control\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4B1876-DC07-494E-8E39-AE182D556B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1292C63-324D-4241-A2CA-A6874F5DE2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11685" yWindow="390" windowWidth="19590" windowHeight="9360" xr2:uid="{C8C1D8BB-10F7-49BF-8560-67C50CB8DDC5}"/>
+    <workbookView xWindow="4410" yWindow="390" windowWidth="19590" windowHeight="9360" xr2:uid="{C8C1D8BB-10F7-49BF-8560-67C50CB8DDC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="88">
   <si>
     <t>No</t>
   </si>
@@ -289,6 +289,18 @@
   </si>
   <si>
     <t>https://shopee.sg/3S-15A-Li-ion-Lithium-Battery-18650-Charger-PCB-BMS-Protection-Board-11.1V-12V-12.6V-Lipo-Cell-Module-i.161750523.6550111605?position=21</t>
+  </si>
+  <si>
+    <t>SB608ZZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required </t>
+  </si>
+  <si>
+    <t>https://sg.misumi-ec.com/vona2/detail/110302273360/?HissuCode=SB608ZZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protects components, ensures smooth and efficent operation </t>
   </si>
 </sst>
 </file>
@@ -784,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8182256-954F-4F59-85A5-CC571E5460A2}">
   <dimension ref="A1:L162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,10 +1639,33 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="3">
+        <v>6.2</v>
+      </c>
       <c r="G27" s="3">
         <f t="shared" ref="G27:G31" si="1">D27*F27</f>
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1684,7 +1719,7 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13">
         <f>SUM(G2:G31)</f>
-        <v>204.46</v>
+        <v>266.46000000000004</v>
       </c>
       <c r="H32" s="18"/>
       <c r="K32" s="14"/>

</xml_diff>